<commit_message>
eod trade analysis done
</commit_message>
<xml_diff>
--- a/angelapi/tradebook.xlsx
+++ b/angelapi/tradebook.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SrvZ\Desktop\Projects\NSE Data\NSE_Data\angelapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DC477C-951A-4D07-9B48-AD703DBD2309}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B3389B-C5E6-4A04-8B62-BDDAD5317424}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
     <sheet name="Pivot" sheetId="4" r:id="rId3"/>
     <sheet name="Formatted" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Raw!$A$2:$Y$389</definedName>
@@ -25,7 +26,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +34,7 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}">
       <x15:timelineCacheRefs>
-        <x15:timelineCacheRef r:id="rId6"/>
+        <x15:timelineCacheRef r:id="rId7"/>
       </x15:timelineCacheRefs>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6212" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6230" uniqueCount="73">
   <si>
     <t>[Trade</t>
   </si>
@@ -245,6 +246,60 @@
   </si>
   <si>
     <t>33300PE</t>
+  </si>
+  <si>
+    <t>[2021-04-19 09:30:00+05:30] SL: -83.3 trade side: CE entry: 30699.4 exit: 30616.1</t>
+  </si>
+  <si>
+    <t>[2021-04-19 09:35:00+05:30] SL: -138.25 trade side: CE entry: 30616.1 exit: 30477.85</t>
+  </si>
+  <si>
+    <t>[2021-04-19 09:55:00+05:30] PnL: 118.95 trade side: CE entry: 30477.85 exit: 30596.8</t>
+  </si>
+  <si>
+    <t>[2021-04-19 10:10:00+05:30] SL: 64.85 trade side: PE entry: 30596.8 exit: 30661.65</t>
+  </si>
+  <si>
+    <t>[2021-04-19 10:20:00+05:30] SL: 68.35 trade side: PE entry: 30563.35 exit: 30631.7</t>
+  </si>
+  <si>
+    <t>[2021-04-19 10:30:00+05:30] SL: 64.4 trade side: PE entry: 30640.2 exit: 30704.6</t>
+  </si>
+  <si>
+    <t>[2021-04-19 10:40:00+05:30] SL: -66.15 trade side: CE entry: 30788.9 exit: 30722.75</t>
+  </si>
+  <si>
+    <t>[2021-04-19 10:50:00+05:30] SL: 70.05 trade side: PE entry: 30722.7 exit: 30792.75</t>
+  </si>
+  <si>
+    <t>[2021-04-19 11:15:00+05:30] SL: -135.55 trade side: CE entry: 30787.9 exit: 30652.35</t>
+  </si>
+  <si>
+    <t>[2021-04-19 11:30:00+05:30] SL: -50.4 trade side: CE entry: 30652.35 exit: 30601.95</t>
+  </si>
+  <si>
+    <t>[2021-04-19 11:50:00+05:30] SL: 66.65 trade side: PE entry: 30601.95 exit: 30668.6</t>
+  </si>
+  <si>
+    <t>[2021-04-19 12:55:00+05:30] PnL: 117.85 trade side: CE entry: 30632.75 exit: 30750.6</t>
+  </si>
+  <si>
+    <t>[2021-04-19 13:20:00+05:30] SL: 53.35 trade side: PE entry: 30764.45 exit: 30817.8</t>
+  </si>
+  <si>
+    <t>[2021-04-19 13:55:00+05:30] PnL: 179.15 trade side: CE entry: 30771.35 exit: 30950.5</t>
+  </si>
+  <si>
+    <t>[2021-04-19 14:15:00+05:30] SL: -67.05 trade side: CE entry: 30958.7 exit: 30891.65</t>
+  </si>
+  <si>
+    <t>[2021-04-19 15:00:00+05:30] PnL: 244.45 trade side: CE entry: 30938.75 exit: 31183.2</t>
+  </si>
+  <si>
+    <t>[2021-04-19 15:15:00+05:30] SL: 68.15 trade side: PE entry: 31211.65 exit: 31279.8</t>
+  </si>
+  <si>
+    <t>[2021-04-19 15:25:00+05:30] SL: -55.25 trade side: CE entry: 31261.85 exit: 31206.6</t>
   </si>
 </sst>
 </file>
@@ -427,8 +482,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" Requires="tsle">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
+      <mc:Choice Requires="tsle">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Date 1">
@@ -446,12 +501,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2012/timeslicer">
-              <tsle:timeslicer xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" name="Date 1"/>
+              <tsle:timeslicer name="Date 1"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -6567,7 +6622,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACC1E03E-3DAE-4993-B5A0-1D60A3CCD91E}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACC1E03E-3DAE-4993-B5A0-1D60A3CCD91E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0">
@@ -42829,7 +42884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129625A4-0EF5-4512-97D8-4C3BEB07A854}">
   <dimension ref="A3:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -50566,7 +50621,7 @@
         <v>35394.9</v>
       </c>
       <c r="I195" s="10">
-        <f t="shared" ref="I195:I258" si="3">A195+B195</f>
+        <f t="shared" ref="I195:I256" si="3">A195+B195</f>
         <v>44249.564525462964</v>
       </c>
     </row>
@@ -61024,4 +61079,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68D4E1A-9C39-48D2-A2D1-6FDC34FA4C18}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="72.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>